<commit_message>
Autaliza os processos na pasta DATA e DATARAW IPSEMG
</commit_message>
<xml_diff>
--- a/data-raw/compras-coronavirus.xlsx
+++ b/data-raw/compras-coronavirus.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3420" uniqueCount="559">
   <si>
     <t>Número Processo -  Formatado</t>
   </si>
@@ -1308,6 +1308,24 @@
   </si>
   <si>
     <t>FILTRO PARA SISTEMA RESPIRATORIO - APLICACAO: ANESTESIA GERAL E VENTILACAO MECANICA; TIPO: ADULTO;</t>
+  </si>
+  <si>
+    <t>2012015 000071/2020</t>
+  </si>
+  <si>
+    <t>Reagentes, Calibradores e Controles para realização de determinação qualitativa de anticorpos tipo IgG para SARS-COV-2 (coronavírus)</t>
+  </si>
+  <si>
+    <t>https://www1.compras.mg.gov.br/contrato/gestaocontratos/arquivosContrato.html?idContrato=163567</t>
+  </si>
+  <si>
+    <t>56.998.701/0032-12</t>
+  </si>
+  <si>
+    <t>ABBOTT LABORATORIOS DO BRASIL LTDA</t>
+  </si>
+  <si>
+    <t>TESTE PARA IMUNODIAGNOSTICO SARS-COV-2 - APLICACAO: DETECCAO QUALITATIVA ANTICORPOS IGG P/ SARS-COV-2; METODO: QUIMIOLUMINESCENCIA; AMOSTRAS: SORO E PLASMA HUMANO;</t>
   </si>
   <si>
     <t>2121022 000013/2020</t>
@@ -1863,7 +1881,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF212"/>
+  <dimension ref="A1:AF213"/>
   <cols>
     <col min="1" max="1" width="27.8093" customWidth="1"/>
     <col min="2" max="2" width="23.8165" customWidth="1"/>
@@ -16830,7 +16848,7 @@
         <v>33</v>
       </c>
       <c r="C165" s="14">
-        <v>43907</v>
+        <v>43987</v>
       </c>
       <c r="D165" s="15" t="s">
         <v>434</v>
@@ -16839,32 +16857,44 @@
         <v>33</v>
       </c>
       <c r="F165" s="16">
-        <v>2120</v>
+        <v>2010</v>
       </c>
       <c r="G165" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="H165" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I165" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="J165" s="17">
+        <v>9.251266e6</v>
+      </c>
+      <c r="K165" s="15" t="s">
         <v>435</v>
       </c>
-      <c r="H165" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I165" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="J165" s="17">
-        <v>0</v>
-      </c>
-      <c r="K165" s="15"/>
-      <c r="L165" s="17"/>
-      <c r="M165" s="15"/>
-      <c r="N165" s="18"/>
-      <c r="O165" s="18"/>
+      <c r="L165" s="17">
+        <v>2010</v>
+      </c>
+      <c r="M165" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="N165" s="18">
+        <v>44013</v>
+      </c>
+      <c r="O165" s="18">
+        <v>44013</v>
+      </c>
       <c r="P165" s="19"/>
-      <c r="Q165" s="18"/>
+      <c r="Q165" s="18">
+        <v>44192</v>
+      </c>
       <c r="R165" s="15" t="s">
-        <v>226</v>
+        <v>436</v>
       </c>
       <c r="S165" s="15" t="s">
-        <v>227</v>
+        <v>437</v>
       </c>
       <c r="T165" s="13" t="s">
         <v>33</v>
@@ -16873,42 +16903,42 @@
         <v>33</v>
       </c>
       <c r="V165" s="17">
-        <v>1.669486e6</v>
+        <v>1.758276e6</v>
       </c>
       <c r="W165" s="15" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="X165" s="17">
-        <v>2121</v>
+        <v>2011</v>
       </c>
       <c r="Y165" s="15" t="s">
-        <v>437</v>
+        <v>412</v>
       </c>
       <c r="Z165" s="15" t="s">
-        <v>438</v>
+        <v>387</v>
       </c>
       <c r="AA165" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB165" s="21">
-        <v>300</v>
+        <v>3000</v>
       </c>
       <c r="AC165" s="22">
-        <v>7.5</v>
+        <v>40.27</v>
       </c>
       <c r="AD165" s="22">
-        <v>7.5</v>
+        <v>40.27</v>
       </c>
       <c r="AE165" s="23">
-        <v>2250</v>
+        <v>120810</v>
       </c>
       <c r="AF165" s="23">
-        <v>2250</v>
+        <v>120810</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A166" s="3" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="B166" s="3" t="s">
         <v>33</v>
@@ -16917,7 +16947,7 @@
         <v>43907</v>
       </c>
       <c r="D166" s="5" t="s">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="E166" s="5" t="s">
         <v>33</v>
@@ -16926,7 +16956,7 @@
         <v>2120</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H166" s="3" t="s">
         <v>36</v>
@@ -16957,51 +16987,51 @@
         <v>33</v>
       </c>
       <c r="V166" s="7">
-        <v>1.696041e6</v>
+        <v>1.669486e6</v>
       </c>
       <c r="W166" s="5" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="X166" s="7">
         <v>2121</v>
       </c>
       <c r="Y166" s="5" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z166" s="5" t="s">
-        <v>135</v>
+        <v>444</v>
       </c>
       <c r="AA166" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB166" s="10">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="AC166" s="11">
-        <v>144</v>
+        <v>7.5</v>
       </c>
       <c r="AD166" s="11">
-        <v>80</v>
+        <v>7.5</v>
       </c>
       <c r="AE166" s="12">
-        <v>14400</v>
+        <v>2250</v>
       </c>
       <c r="AF166" s="12">
-        <v>8000</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A167" s="13" t="s">
+        <v>439</v>
+      </c>
+      <c r="B167" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C167" s="14">
+        <v>43907</v>
+      </c>
+      <c r="D167" s="15" t="s">
         <v>440</v>
-      </c>
-      <c r="B167" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C167" s="14">
-        <v>43908</v>
-      </c>
-      <c r="D167" s="15" t="s">
-        <v>441</v>
       </c>
       <c r="E167" s="15" t="s">
         <v>33</v>
@@ -17010,85 +17040,73 @@
         <v>2120</v>
       </c>
       <c r="G167" s="13" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H167" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I167" s="13" t="s">
-        <v>442</v>
+        <v>138</v>
       </c>
       <c r="J167" s="17">
-        <v>9.246044e6</v>
-      </c>
-      <c r="K167" s="15" t="s">
-        <v>443</v>
-      </c>
-      <c r="L167" s="17">
-        <v>2120</v>
-      </c>
-      <c r="M167" s="15" t="s">
-        <v>435</v>
-      </c>
-      <c r="N167" s="18">
-        <v>43976</v>
-      </c>
-      <c r="O167" s="18">
-        <v>43946</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K167" s="15"/>
+      <c r="L167" s="17"/>
+      <c r="M167" s="15"/>
+      <c r="N167" s="18"/>
+      <c r="O167" s="18"/>
       <c r="P167" s="19"/>
-      <c r="Q167" s="18">
-        <v>44196</v>
-      </c>
+      <c r="Q167" s="18"/>
       <c r="R167" s="15" t="s">
-        <v>444</v>
+        <v>226</v>
       </c>
       <c r="S167" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="T167" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U167" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V167" s="17">
+        <v>1.696041e6</v>
+      </c>
+      <c r="W167" s="15" t="s">
         <v>445</v>
-      </c>
-      <c r="T167" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U167" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V167" s="17">
-        <v>1.66937e6</v>
-      </c>
-      <c r="W167" s="15" t="s">
-        <v>193</v>
       </c>
       <c r="X167" s="17">
         <v>2121</v>
       </c>
       <c r="Y167" s="15" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z167" s="15" t="s">
         <v>135</v>
       </c>
       <c r="AA167" s="13" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="AB167" s="21">
-        <v>700</v>
+        <v>100</v>
       </c>
       <c r="AC167" s="22">
-        <v>6.58</v>
+        <v>144</v>
       </c>
       <c r="AD167" s="22">
-        <v>6.58</v>
+        <v>80</v>
       </c>
       <c r="AE167" s="23">
-        <v>4606</v>
+        <v>14400</v>
       </c>
       <c r="AF167" s="23">
-        <v>4606</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A168" s="3" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="B168" s="3" t="s">
         <v>33</v>
@@ -17097,7 +17115,7 @@
         <v>43908</v>
       </c>
       <c r="D168" s="5" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E168" s="5" t="s">
         <v>33</v>
@@ -17106,25 +17124,25 @@
         <v>2120</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H168" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="J168" s="7">
         <v>9.246044e6</v>
       </c>
       <c r="K168" s="5" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L168" s="7">
         <v>2120</v>
       </c>
       <c r="M168" s="5" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="N168" s="8">
         <v>43976</v>
@@ -17137,10 +17155,10 @@
         <v>44196</v>
       </c>
       <c r="R168" s="5" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="S168" s="5" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="T168" s="3" t="s">
         <v>33</v>
@@ -17149,16 +17167,16 @@
         <v>33</v>
       </c>
       <c r="V168" s="7">
-        <v>1.669397e6</v>
+        <v>1.66937e6</v>
       </c>
       <c r="W168" s="5" t="s">
-        <v>446</v>
+        <v>193</v>
       </c>
       <c r="X168" s="7">
         <v>2121</v>
       </c>
       <c r="Y168" s="5" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z168" s="5" t="s">
         <v>135</v>
@@ -17167,24 +17185,24 @@
         <v>123</v>
       </c>
       <c r="AB168" s="10">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="AC168" s="11">
-        <v>6.8</v>
+        <v>6.58</v>
       </c>
       <c r="AD168" s="11">
-        <v>6.8</v>
+        <v>6.58</v>
       </c>
       <c r="AE168" s="12">
-        <v>1360</v>
+        <v>4606</v>
       </c>
       <c r="AF168" s="12">
-        <v>1360</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A169" s="13" t="s">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="B169" s="13" t="s">
         <v>33</v>
@@ -17193,7 +17211,7 @@
         <v>43908</v>
       </c>
       <c r="D169" s="15" t="s">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E169" s="15" t="s">
         <v>33</v>
@@ -17202,25 +17220,25 @@
         <v>2120</v>
       </c>
       <c r="G169" s="13" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H169" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I169" s="13" t="s">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="J169" s="17">
         <v>9.246044e6</v>
       </c>
       <c r="K169" s="15" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L169" s="17">
         <v>2120</v>
       </c>
       <c r="M169" s="15" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="N169" s="18">
         <v>43976</v>
@@ -17233,10 +17251,10 @@
         <v>44196</v>
       </c>
       <c r="R169" s="15" t="s">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="S169" s="15" t="s">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="T169" s="13" t="s">
         <v>33</v>
@@ -17245,51 +17263,51 @@
         <v>33</v>
       </c>
       <c r="V169" s="17">
-        <v>1.669486e6</v>
+        <v>1.669397e6</v>
       </c>
       <c r="W169" s="15" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="X169" s="17">
         <v>2121</v>
       </c>
       <c r="Y169" s="15" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z169" s="15" t="s">
-        <v>438</v>
+        <v>135</v>
       </c>
       <c r="AA169" s="13" t="s">
         <v>123</v>
       </c>
       <c r="AB169" s="21">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="AC169" s="22">
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="AD169" s="22">
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="AE169" s="23">
-        <v>400</v>
+        <v>1360</v>
       </c>
       <c r="AF169" s="23">
-        <v>400</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A170" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C170" s="4">
+        <v>43908</v>
+      </c>
+      <c r="D170" s="5" t="s">
         <v>447</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C170" s="4">
-        <v>43909</v>
-      </c>
-      <c r="D170" s="5" t="s">
-        <v>448</v>
       </c>
       <c r="E170" s="5" t="s">
         <v>33</v>
@@ -17298,29 +17316,41 @@
         <v>2120</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H170" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>138</v>
+        <v>448</v>
       </c>
       <c r="J170" s="7">
-        <v>0</v>
-      </c>
-      <c r="K170" s="5"/>
-      <c r="L170" s="7"/>
-      <c r="M170" s="5"/>
-      <c r="N170" s="8"/>
-      <c r="O170" s="8"/>
+        <v>9.246044e6</v>
+      </c>
+      <c r="K170" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="L170" s="7">
+        <v>2120</v>
+      </c>
+      <c r="M170" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="N170" s="8">
+        <v>43976</v>
+      </c>
+      <c r="O170" s="8">
+        <v>43946</v>
+      </c>
       <c r="P170" s="9"/>
-      <c r="Q170" s="8"/>
+      <c r="Q170" s="8">
+        <v>44196</v>
+      </c>
       <c r="R170" s="5" t="s">
-        <v>226</v>
+        <v>450</v>
       </c>
       <c r="S170" s="5" t="s">
-        <v>227</v>
+        <v>451</v>
       </c>
       <c r="T170" s="3" t="s">
         <v>33</v>
@@ -17329,51 +17359,51 @@
         <v>33</v>
       </c>
       <c r="V170" s="7">
-        <v>513830</v>
+        <v>1.669486e6</v>
       </c>
       <c r="W170" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="X170" s="7">
         <v>2121</v>
       </c>
       <c r="Y170" s="5" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z170" s="5" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="AA170" s="3" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="AB170" s="10">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="AC170" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AD170" s="11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AE170" s="12">
-        <v>1050</v>
+        <v>400</v>
       </c>
       <c r="AF170" s="12">
-        <v>1050</v>
+        <v>400</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A171" s="13" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B171" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C171" s="14">
-        <v>43915</v>
+        <v>43909</v>
       </c>
       <c r="D171" s="15" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="E171" s="15" t="s">
         <v>33</v>
@@ -17382,7 +17412,7 @@
         <v>2120</v>
       </c>
       <c r="G171" s="13" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H171" s="13" t="s">
         <v>36</v>
@@ -17413,51 +17443,51 @@
         <v>33</v>
       </c>
       <c r="V171" s="17">
-        <v>1.69216e6</v>
+        <v>513830</v>
       </c>
       <c r="W171" s="15" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="X171" s="17">
         <v>2121</v>
       </c>
       <c r="Y171" s="15" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z171" s="15" t="s">
-        <v>135</v>
+        <v>456</v>
       </c>
       <c r="AA171" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB171" s="21">
-        <v>40</v>
+        <v>210</v>
       </c>
       <c r="AC171" s="22">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="AD171" s="22">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="AE171" s="23">
-        <v>1600</v>
+        <v>1050</v>
       </c>
       <c r="AF171" s="23">
-        <v>1600</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A172" s="3" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="B172" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C172" s="4">
-        <v>43938</v>
+        <v>43915</v>
       </c>
       <c r="D172" s="5" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="E172" s="5" t="s">
         <v>33</v>
@@ -17466,41 +17496,29 @@
         <v>2120</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H172" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="J172" s="7">
-        <v>9.246007e6</v>
-      </c>
-      <c r="K172" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="L172" s="7">
-        <v>2120</v>
-      </c>
-      <c r="M172" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="N172" s="8">
-        <v>43944</v>
-      </c>
-      <c r="O172" s="8">
-        <v>43944</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K172" s="5"/>
+      <c r="L172" s="7"/>
+      <c r="M172" s="5"/>
+      <c r="N172" s="8"/>
+      <c r="O172" s="8"/>
       <c r="P172" s="9"/>
-      <c r="Q172" s="8">
-        <v>44126</v>
-      </c>
+      <c r="Q172" s="8"/>
       <c r="R172" s="5" t="s">
-        <v>457</v>
+        <v>226</v>
       </c>
       <c r="S172" s="5" t="s">
-        <v>458</v>
+        <v>227</v>
       </c>
       <c r="T172" s="3" t="s">
         <v>33</v>
@@ -17509,7 +17527,7 @@
         <v>33</v>
       </c>
       <c r="V172" s="7">
-        <v>1.71894e6</v>
+        <v>1.69216e6</v>
       </c>
       <c r="W172" s="5" t="s">
         <v>459</v>
@@ -17518,28 +17536,28 @@
         <v>2121</v>
       </c>
       <c r="Y172" s="5" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z172" s="5" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="AA172" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB172" s="10">
-        <v>84000</v>
+        <v>40</v>
       </c>
       <c r="AC172" s="11">
-        <v>2.2</v>
+        <v>40</v>
       </c>
       <c r="AD172" s="11">
-        <v>1.71</v>
+        <v>40</v>
       </c>
       <c r="AE172" s="12">
-        <v>184800</v>
+        <v>1600</v>
       </c>
       <c r="AF172" s="12">
-        <v>143640</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -17550,7 +17568,7 @@
         <v>33</v>
       </c>
       <c r="C173" s="14">
-        <v>43986</v>
+        <v>43938</v>
       </c>
       <c r="D173" s="15" t="s">
         <v>461</v>
@@ -17562,29 +17580,41 @@
         <v>2120</v>
       </c>
       <c r="G173" s="13" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H173" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I173" s="13" t="s">
-        <v>138</v>
+        <v>37</v>
       </c>
       <c r="J173" s="17">
-        <v>0</v>
-      </c>
-      <c r="K173" s="15"/>
-      <c r="L173" s="17"/>
-      <c r="M173" s="15"/>
-      <c r="N173" s="18"/>
-      <c r="O173" s="18"/>
+        <v>9.246007e6</v>
+      </c>
+      <c r="K173" s="15" t="s">
+        <v>462</v>
+      </c>
+      <c r="L173" s="17">
+        <v>2120</v>
+      </c>
+      <c r="M173" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="N173" s="18">
+        <v>43944</v>
+      </c>
+      <c r="O173" s="18">
+        <v>43944</v>
+      </c>
       <c r="P173" s="19"/>
-      <c r="Q173" s="18"/>
+      <c r="Q173" s="18">
+        <v>44126</v>
+      </c>
       <c r="R173" s="15" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="S173" s="15" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="T173" s="13" t="s">
         <v>33</v>
@@ -17593,42 +17623,42 @@
         <v>33</v>
       </c>
       <c r="V173" s="17">
-        <v>50245</v>
+        <v>1.71894e6</v>
       </c>
       <c r="W173" s="15" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="X173" s="17">
         <v>2121</v>
       </c>
       <c r="Y173" s="15" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z173" s="15" t="s">
-        <v>438</v>
+        <v>122</v>
       </c>
       <c r="AA173" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB173" s="21">
-        <v>200</v>
+        <v>84000</v>
       </c>
       <c r="AC173" s="22">
-        <v>1.9131</v>
+        <v>2.2</v>
       </c>
       <c r="AD173" s="22">
-        <v>1.84</v>
+        <v>1.71</v>
       </c>
       <c r="AE173" s="23">
-        <v>382.62</v>
+        <v>184800</v>
       </c>
       <c r="AF173" s="23">
-        <v>368</v>
+        <v>143640</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A174" s="3" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B174" s="3" t="s">
         <v>33</v>
@@ -17637,7 +17667,7 @@
         <v>43986</v>
       </c>
       <c r="D174" s="5" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="E174" s="5" t="s">
         <v>33</v>
@@ -17646,7 +17676,7 @@
         <v>2120</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="H174" s="3" t="s">
         <v>36</v>
@@ -17665,10 +17695,10 @@
       <c r="P174" s="9"/>
       <c r="Q174" s="8"/>
       <c r="R174" s="5" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="S174" s="5" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="T174" s="3" t="s">
         <v>33</v>
@@ -17677,37 +17707,37 @@
         <v>33</v>
       </c>
       <c r="V174" s="7">
-        <v>835889</v>
+        <v>50245</v>
       </c>
       <c r="W174" s="5" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="X174" s="7">
         <v>2121</v>
       </c>
       <c r="Y174" s="5" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="Z174" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA174" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB174" s="10">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="AC174" s="11">
-        <v>24</v>
+        <v>1.9131</v>
       </c>
       <c r="AD174" s="11">
-        <v>32.87</v>
+        <v>1.84</v>
       </c>
       <c r="AE174" s="12">
-        <v>720</v>
+        <v>382.62</v>
       </c>
       <c r="AF174" s="12">
-        <v>986.1</v>
+        <v>368</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="1" ht="18.1322" customHeight="1">
@@ -17718,7 +17748,7 @@
         <v>33</v>
       </c>
       <c r="C175" s="14">
-        <v>43920</v>
+        <v>43986</v>
       </c>
       <c r="D175" s="15" t="s">
         <v>467</v>
@@ -17727,16 +17757,16 @@
         <v>33</v>
       </c>
       <c r="F175" s="16">
-        <v>2260</v>
+        <v>2120</v>
       </c>
       <c r="G175" s="13" t="s">
-        <v>468</v>
+        <v>441</v>
       </c>
       <c r="H175" s="13" t="s">
         <v>36</v>
       </c>
       <c r="I175" s="13" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="J175" s="17">
         <v>0</v>
@@ -17749,11 +17779,11 @@
       <c r="P175" s="19"/>
       <c r="Q175" s="18"/>
       <c r="R175" s="15" t="s">
+        <v>468</v>
+      </c>
+      <c r="S175" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="S175" s="15" t="s">
-        <v>470</v>
-      </c>
       <c r="T175" s="13" t="s">
         <v>33</v>
       </c>
@@ -17761,42 +17791,42 @@
         <v>33</v>
       </c>
       <c r="V175" s="17">
-        <v>82414</v>
+        <v>835889</v>
       </c>
       <c r="W175" s="15" t="s">
         <v>471</v>
       </c>
       <c r="X175" s="17">
-        <v>2261</v>
+        <v>2121</v>
       </c>
       <c r="Y175" s="15" t="s">
-        <v>468</v>
+        <v>443</v>
       </c>
       <c r="Z175" s="15" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="AA175" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB175" s="21">
-        <v>10000</v>
+        <v>30</v>
       </c>
       <c r="AC175" s="22">
-        <v>676000e-6</v>
+        <v>24</v>
       </c>
       <c r="AD175" s="22">
-        <v>676000e-6</v>
+        <v>32.87</v>
       </c>
       <c r="AE175" s="23">
-        <v>6760</v>
+        <v>720</v>
       </c>
       <c r="AF175" s="23">
-        <v>6760</v>
+        <v>986.1</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A176" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B176" s="3" t="s">
         <v>33</v>
@@ -17805,7 +17835,7 @@
         <v>43920</v>
       </c>
       <c r="D176" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E176" s="5" t="s">
         <v>33</v>
@@ -17814,7 +17844,7 @@
         <v>2260</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H176" s="3" t="s">
         <v>36</v>
@@ -17833,10 +17863,10 @@
       <c r="P176" s="9"/>
       <c r="Q176" s="8"/>
       <c r="R176" s="5" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="S176" s="5" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="T176" s="3" t="s">
         <v>33</v>
@@ -17845,42 +17875,42 @@
         <v>33</v>
       </c>
       <c r="V176" s="7">
-        <v>1.670891e6</v>
+        <v>82414</v>
       </c>
       <c r="W176" s="5" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="X176" s="7">
         <v>2261</v>
       </c>
       <c r="Y176" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z176" s="5" t="s">
-        <v>122</v>
+        <v>387</v>
       </c>
       <c r="AA176" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB176" s="10">
-        <v>20</v>
+        <v>10000</v>
       </c>
       <c r="AC176" s="11">
-        <v>34.9</v>
+        <v>676000e-6</v>
       </c>
       <c r="AD176" s="11">
-        <v>34.9</v>
+        <v>676000e-6</v>
       </c>
       <c r="AE176" s="12">
-        <v>698</v>
+        <v>6760</v>
       </c>
       <c r="AF176" s="12">
-        <v>698</v>
+        <v>6760</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A177" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B177" s="13" t="s">
         <v>33</v>
@@ -17889,7 +17919,7 @@
         <v>43920</v>
       </c>
       <c r="D177" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E177" s="15" t="s">
         <v>33</v>
@@ -17898,7 +17928,7 @@
         <v>2260</v>
       </c>
       <c r="G177" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H177" s="13" t="s">
         <v>36</v>
@@ -17917,10 +17947,10 @@
       <c r="P177" s="19"/>
       <c r="Q177" s="18"/>
       <c r="R177" s="15" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="S177" s="15" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="T177" s="13" t="s">
         <v>33</v>
@@ -17929,42 +17959,42 @@
         <v>33</v>
       </c>
       <c r="V177" s="17">
-        <v>1.69773e6</v>
+        <v>1.670891e6</v>
       </c>
       <c r="W177" s="15" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="X177" s="17">
         <v>2261</v>
       </c>
       <c r="Y177" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z177" s="15" t="s">
-        <v>387</v>
+        <v>122</v>
       </c>
       <c r="AA177" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB177" s="21">
-        <v>20000</v>
+        <v>20</v>
       </c>
       <c r="AC177" s="22">
-        <v>12.43</v>
+        <v>34.9</v>
       </c>
       <c r="AD177" s="22">
-        <v>12.43</v>
+        <v>34.9</v>
       </c>
       <c r="AE177" s="23">
-        <v>248600</v>
+        <v>698</v>
       </c>
       <c r="AF177" s="23">
-        <v>248600</v>
+        <v>698</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A178" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B178" s="3" t="s">
         <v>33</v>
@@ -17973,7 +18003,7 @@
         <v>43920</v>
       </c>
       <c r="D178" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E178" s="5" t="s">
         <v>33</v>
@@ -17982,7 +18012,7 @@
         <v>2260</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H178" s="3" t="s">
         <v>36</v>
@@ -18001,10 +18031,10 @@
       <c r="P178" s="9"/>
       <c r="Q178" s="8"/>
       <c r="R178" s="5" t="s">
-        <v>384</v>
+        <v>479</v>
       </c>
       <c r="S178" s="5" t="s">
-        <v>385</v>
+        <v>480</v>
       </c>
       <c r="T178" s="3" t="s">
         <v>33</v>
@@ -18013,16 +18043,16 @@
         <v>33</v>
       </c>
       <c r="V178" s="7">
-        <v>394890</v>
+        <v>1.69773e6</v>
       </c>
       <c r="W178" s="5" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="X178" s="7">
         <v>2261</v>
       </c>
       <c r="Y178" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z178" s="5" t="s">
         <v>387</v>
@@ -18031,24 +18061,24 @@
         <v>44</v>
       </c>
       <c r="AB178" s="10">
-        <v>450</v>
+        <v>20000</v>
       </c>
       <c r="AC178" s="11">
-        <v>7.98</v>
+        <v>12.43</v>
       </c>
       <c r="AD178" s="11">
-        <v>7.98</v>
+        <v>12.43</v>
       </c>
       <c r="AE178" s="12">
-        <v>3591</v>
+        <v>248600</v>
       </c>
       <c r="AF178" s="12">
-        <v>3591</v>
+        <v>248600</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A179" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B179" s="13" t="s">
         <v>33</v>
@@ -18057,7 +18087,7 @@
         <v>43920</v>
       </c>
       <c r="D179" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E179" s="15" t="s">
         <v>33</v>
@@ -18066,7 +18096,7 @@
         <v>2260</v>
       </c>
       <c r="G179" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H179" s="13" t="s">
         <v>36</v>
@@ -18097,16 +18127,16 @@
         <v>33</v>
       </c>
       <c r="V179" s="17">
-        <v>1.368818e6</v>
+        <v>394890</v>
       </c>
       <c r="W179" s="15" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="X179" s="17">
         <v>2261</v>
       </c>
       <c r="Y179" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z179" s="15" t="s">
         <v>387</v>
@@ -18115,24 +18145,24 @@
         <v>44</v>
       </c>
       <c r="AB179" s="21">
-        <v>10</v>
+        <v>450</v>
       </c>
       <c r="AC179" s="22">
-        <v>293.6</v>
+        <v>7.98</v>
       </c>
       <c r="AD179" s="22">
-        <v>293.6</v>
+        <v>7.98</v>
       </c>
       <c r="AE179" s="23">
-        <v>2936</v>
+        <v>3591</v>
       </c>
       <c r="AF179" s="23">
-        <v>2936</v>
+        <v>3591</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A180" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B180" s="3" t="s">
         <v>33</v>
@@ -18141,7 +18171,7 @@
         <v>43920</v>
       </c>
       <c r="D180" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E180" s="5" t="s">
         <v>33</v>
@@ -18150,7 +18180,7 @@
         <v>2260</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H180" s="3" t="s">
         <v>36</v>
@@ -18181,16 +18211,16 @@
         <v>33</v>
       </c>
       <c r="V180" s="7">
-        <v>1.497391e6</v>
+        <v>1.368818e6</v>
       </c>
       <c r="W180" s="5" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="X180" s="7">
         <v>2261</v>
       </c>
       <c r="Y180" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z180" s="5" t="s">
         <v>387</v>
@@ -18199,24 +18229,24 @@
         <v>44</v>
       </c>
       <c r="AB180" s="10">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AC180" s="11">
-        <v>3420</v>
+        <v>293.6</v>
       </c>
       <c r="AD180" s="11">
-        <v>3420</v>
+        <v>293.6</v>
       </c>
       <c r="AE180" s="12">
-        <v>51300</v>
+        <v>2936</v>
       </c>
       <c r="AF180" s="12">
-        <v>51300</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A181" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B181" s="13" t="s">
         <v>33</v>
@@ -18225,7 +18255,7 @@
         <v>43920</v>
       </c>
       <c r="D181" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E181" s="15" t="s">
         <v>33</v>
@@ -18234,7 +18264,7 @@
         <v>2260</v>
       </c>
       <c r="G181" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H181" s="13" t="s">
         <v>36</v>
@@ -18253,10 +18283,10 @@
       <c r="P181" s="19"/>
       <c r="Q181" s="18"/>
       <c r="R181" s="15" t="s">
-        <v>479</v>
+        <v>384</v>
       </c>
       <c r="S181" s="15" t="s">
-        <v>480</v>
+        <v>385</v>
       </c>
       <c r="T181" s="13" t="s">
         <v>33</v>
@@ -18265,16 +18295,16 @@
         <v>33</v>
       </c>
       <c r="V181" s="17">
-        <v>1.669613e6</v>
+        <v>1.497391e6</v>
       </c>
       <c r="W181" s="15" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="X181" s="17">
         <v>2261</v>
       </c>
       <c r="Y181" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z181" s="15" t="s">
         <v>387</v>
@@ -18283,24 +18313,24 @@
         <v>44</v>
       </c>
       <c r="AB181" s="21">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="AC181" s="22">
-        <v>31.96</v>
+        <v>3420</v>
       </c>
       <c r="AD181" s="22">
-        <v>31.96</v>
+        <v>3420</v>
       </c>
       <c r="AE181" s="23">
-        <v>319.6</v>
+        <v>51300</v>
       </c>
       <c r="AF181" s="23">
-        <v>319.6</v>
+        <v>51300</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A182" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B182" s="3" t="s">
         <v>33</v>
@@ -18309,7 +18339,7 @@
         <v>43920</v>
       </c>
       <c r="D182" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E182" s="5" t="s">
         <v>33</v>
@@ -18318,7 +18348,7 @@
         <v>2260</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H182" s="3" t="s">
         <v>36</v>
@@ -18337,10 +18367,10 @@
       <c r="P182" s="9"/>
       <c r="Q182" s="8"/>
       <c r="R182" s="5" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="S182" s="5" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="T182" s="3" t="s">
         <v>33</v>
@@ -18349,16 +18379,16 @@
         <v>33</v>
       </c>
       <c r="V182" s="7">
-        <v>857025</v>
+        <v>1.669613e6</v>
       </c>
       <c r="W182" s="5" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="X182" s="7">
         <v>2261</v>
       </c>
       <c r="Y182" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z182" s="5" t="s">
         <v>387</v>
@@ -18367,24 +18397,24 @@
         <v>44</v>
       </c>
       <c r="AB182" s="10">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="AC182" s="11">
-        <v>16.756</v>
+        <v>31.96</v>
       </c>
       <c r="AD182" s="11">
-        <v>16.756</v>
+        <v>31.96</v>
       </c>
       <c r="AE182" s="12">
-        <v>1675.6</v>
+        <v>319.6</v>
       </c>
       <c r="AF182" s="12">
-        <v>1675.6</v>
+        <v>319.6</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A183" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B183" s="13" t="s">
         <v>33</v>
@@ -18393,7 +18423,7 @@
         <v>43920</v>
       </c>
       <c r="D183" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E183" s="15" t="s">
         <v>33</v>
@@ -18402,7 +18432,7 @@
         <v>2260</v>
       </c>
       <c r="G183" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H183" s="13" t="s">
         <v>36</v>
@@ -18421,10 +18451,10 @@
       <c r="P183" s="19"/>
       <c r="Q183" s="18"/>
       <c r="R183" s="15" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="S183" s="15" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="T183" s="13" t="s">
         <v>33</v>
@@ -18433,16 +18463,16 @@
         <v>33</v>
       </c>
       <c r="V183" s="17">
-        <v>1.151746e6</v>
+        <v>857025</v>
       </c>
       <c r="W183" s="15" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="X183" s="17">
         <v>2261</v>
       </c>
       <c r="Y183" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z183" s="15" t="s">
         <v>387</v>
@@ -18451,24 +18481,24 @@
         <v>44</v>
       </c>
       <c r="AB183" s="21">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="AC183" s="22">
-        <v>117</v>
+        <v>16.756</v>
       </c>
       <c r="AD183" s="22">
-        <v>117</v>
+        <v>16.756</v>
       </c>
       <c r="AE183" s="23">
-        <v>2340</v>
+        <v>1675.6</v>
       </c>
       <c r="AF183" s="23">
-        <v>2340</v>
+        <v>1675.6</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A184" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B184" s="3" t="s">
         <v>33</v>
@@ -18477,7 +18507,7 @@
         <v>43920</v>
       </c>
       <c r="D184" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E184" s="5" t="s">
         <v>33</v>
@@ -18486,7 +18516,7 @@
         <v>2260</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H184" s="3" t="s">
         <v>36</v>
@@ -18495,32 +18525,20 @@
         <v>37</v>
       </c>
       <c r="J184" s="7">
-        <v>9.245762e6</v>
-      </c>
-      <c r="K184" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="L184" s="7">
-        <v>2260</v>
-      </c>
-      <c r="M184" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="N184" s="8">
-        <v>43936</v>
-      </c>
-      <c r="O184" s="8">
-        <v>43936</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K184" s="5"/>
+      <c r="L184" s="7"/>
+      <c r="M184" s="5"/>
+      <c r="N184" s="8"/>
+      <c r="O184" s="8"/>
       <c r="P184" s="9"/>
-      <c r="Q184" s="8">
-        <v>44115</v>
-      </c>
+      <c r="Q184" s="8"/>
       <c r="R184" s="5" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="S184" s="5" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="T184" s="3" t="s">
         <v>33</v>
@@ -18529,42 +18547,42 @@
         <v>33</v>
       </c>
       <c r="V184" s="7">
-        <v>781673</v>
+        <v>1.151746e6</v>
       </c>
       <c r="W184" s="5" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="X184" s="7">
         <v>2261</v>
       </c>
       <c r="Y184" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z184" s="5" t="s">
-        <v>115</v>
+        <v>387</v>
       </c>
       <c r="AA184" s="3" t="s">
         <v>44</v>
       </c>
       <c r="AB184" s="10">
-        <v>30000</v>
+        <v>20</v>
       </c>
       <c r="AC184" s="11">
-        <v>900000e-6</v>
+        <v>117</v>
       </c>
       <c r="AD184" s="11">
-        <v>900000e-6</v>
+        <v>117</v>
       </c>
       <c r="AE184" s="12">
-        <v>27000</v>
+        <v>2340</v>
       </c>
       <c r="AF184" s="12">
-        <v>27000</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A185" s="13" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B185" s="13" t="s">
         <v>33</v>
@@ -18573,7 +18591,7 @@
         <v>43920</v>
       </c>
       <c r="D185" s="15" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E185" s="15" t="s">
         <v>33</v>
@@ -18582,7 +18600,7 @@
         <v>2260</v>
       </c>
       <c r="G185" s="13" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H185" s="13" t="s">
         <v>36</v>
@@ -18591,16 +18609,16 @@
         <v>37</v>
       </c>
       <c r="J185" s="17">
-        <v>9.245763e6</v>
+        <v>9.245762e6</v>
       </c>
       <c r="K185" s="15" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="L185" s="17">
         <v>2260</v>
       </c>
       <c r="M185" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="N185" s="18">
         <v>43936</v>
@@ -18613,10 +18631,10 @@
         <v>44115</v>
       </c>
       <c r="R185" s="15" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="S185" s="15" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="T185" s="13" t="s">
         <v>33</v>
@@ -18625,16 +18643,16 @@
         <v>33</v>
       </c>
       <c r="V185" s="17">
-        <v>538957</v>
+        <v>781673</v>
       </c>
       <c r="W185" s="15" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
       <c r="X185" s="17">
         <v>2261</v>
       </c>
       <c r="Y185" s="15" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z185" s="15" t="s">
         <v>115</v>
@@ -18646,21 +18664,21 @@
         <v>30000</v>
       </c>
       <c r="AC185" s="22">
-        <v>550000e-6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AD185" s="22">
-        <v>550000e-6</v>
+        <v>900000e-6</v>
       </c>
       <c r="AE185" s="23">
-        <v>16500</v>
+        <v>27000</v>
       </c>
       <c r="AF185" s="23">
-        <v>16500</v>
+        <v>27000</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A186" s="3" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="B186" s="3" t="s">
         <v>33</v>
@@ -18669,7 +18687,7 @@
         <v>43920</v>
       </c>
       <c r="D186" s="5" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="E186" s="5" t="s">
         <v>33</v>
@@ -18678,7 +18696,7 @@
         <v>2260</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="H186" s="3" t="s">
         <v>36</v>
@@ -18690,13 +18708,13 @@
         <v>9.245763e6</v>
       </c>
       <c r="K186" s="5" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="L186" s="7">
         <v>2260</v>
       </c>
       <c r="M186" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="N186" s="8">
         <v>43936</v>
@@ -18709,10 +18727,10 @@
         <v>44115</v>
       </c>
       <c r="R186" s="5" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="S186" s="5" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="T186" s="3" t="s">
         <v>33</v>
@@ -18721,16 +18739,16 @@
         <v>33</v>
       </c>
       <c r="V186" s="7">
-        <v>1.651595e6</v>
+        <v>538957</v>
       </c>
       <c r="W186" s="5" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="X186" s="7">
         <v>2261</v>
       </c>
       <c r="Y186" s="5" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="Z186" s="5" t="s">
         <v>115</v>
@@ -18742,39 +18760,39 @@
         <v>30000</v>
       </c>
       <c r="AC186" s="11">
-        <v>1.08</v>
+        <v>550000e-6</v>
       </c>
       <c r="AD186" s="11">
-        <v>1.08</v>
+        <v>550000e-6</v>
       </c>
       <c r="AE186" s="12">
-        <v>32400</v>
+        <v>16500</v>
       </c>
       <c r="AF186" s="12">
-        <v>32400</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A187" s="13" t="s">
-        <v>497</v>
+        <v>472</v>
       </c>
       <c r="B187" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C187" s="14">
-        <v>43921</v>
+        <v>43920</v>
       </c>
       <c r="D187" s="15" t="s">
-        <v>498</v>
+        <v>473</v>
       </c>
       <c r="E187" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F187" s="16">
-        <v>2300</v>
+        <v>2260</v>
       </c>
       <c r="G187" s="13" t="s">
-        <v>499</v>
+        <v>474</v>
       </c>
       <c r="H187" s="13" t="s">
         <v>36</v>
@@ -18783,87 +18801,85 @@
         <v>37</v>
       </c>
       <c r="J187" s="17">
-        <v>9.245674e6</v>
+        <v>9.245763e6</v>
       </c>
       <c r="K187" s="15" t="s">
+        <v>498</v>
+      </c>
+      <c r="L187" s="17">
+        <v>2260</v>
+      </c>
+      <c r="M187" s="15" t="s">
+        <v>474</v>
+      </c>
+      <c r="N187" s="18">
+        <v>43936</v>
+      </c>
+      <c r="O187" s="18">
+        <v>43936</v>
+      </c>
+      <c r="P187" s="19"/>
+      <c r="Q187" s="18">
+        <v>44115</v>
+      </c>
+      <c r="R187" s="15" t="s">
+        <v>499</v>
+      </c>
+      <c r="S187" s="15" t="s">
         <v>500</v>
       </c>
-      <c r="L187" s="17">
-        <v>2300</v>
-      </c>
-      <c r="M187" s="15" t="s">
-        <v>499</v>
-      </c>
-      <c r="N187" s="18">
-        <v>43922</v>
-      </c>
-      <c r="O187" s="18">
-        <v>43922</v>
-      </c>
-      <c r="P187" s="19">
-        <v>44105</v>
-      </c>
-      <c r="Q187" s="18">
-        <v>44131</v>
-      </c>
-      <c r="R187" s="15" t="s">
-        <v>501</v>
-      </c>
-      <c r="S187" s="15" t="s">
+      <c r="T187" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U187" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="V187" s="17">
+        <v>1.651595e6</v>
+      </c>
+      <c r="W187" s="15" t="s">
         <v>502</v>
       </c>
-      <c r="T187" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="U187" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="V187" s="17">
-        <v>1155</v>
-      </c>
-      <c r="W187" s="15" t="s">
-        <v>107</v>
-      </c>
       <c r="X187" s="17">
-        <v>2301</v>
+        <v>2261</v>
       </c>
       <c r="Y187" s="15" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
       <c r="Z187" s="15" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="AA187" s="13" t="s">
         <v>44</v>
       </c>
       <c r="AB187" s="21">
-        <v>0</v>
+        <v>30000</v>
       </c>
       <c r="AC187" s="22">
-        <v>4.35942886e6</v>
+        <v>1.08</v>
       </c>
       <c r="AD187" s="22">
-        <v>4.35942886e6</v>
+        <v>1.08</v>
       </c>
       <c r="AE187" s="23">
-        <v>4.35942886e6</v>
+        <v>32400</v>
       </c>
       <c r="AF187" s="23">
-        <v>4.35942886e6</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A188" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C188" s="4">
+        <v>43921</v>
+      </c>
+      <c r="D188" s="5" t="s">
         <v>504</v>
-      </c>
-      <c r="B188" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C188" s="4">
-        <v>43935</v>
-      </c>
-      <c r="D188" s="5" t="s">
-        <v>505</v>
       </c>
       <c r="E188" s="5" t="s">
         <v>33</v>
@@ -18872,7 +18888,7 @@
         <v>2300</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="H188" s="3" t="s">
         <v>36</v>
@@ -18881,7 +18897,7 @@
         <v>37</v>
       </c>
       <c r="J188" s="7">
-        <v>9.24595e6</v>
+        <v>9.245674e6</v>
       </c>
       <c r="K188" s="5" t="s">
         <v>506</v>
@@ -18890,19 +18906,19 @@
         <v>2300</v>
       </c>
       <c r="M188" s="5" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="N188" s="8">
-        <v>43936</v>
+        <v>43922</v>
       </c>
       <c r="O188" s="8">
-        <v>43936</v>
+        <v>43922</v>
       </c>
       <c r="P188" s="9">
-        <v>44119</v>
+        <v>44105</v>
       </c>
       <c r="Q188" s="8">
-        <v>44119</v>
+        <v>44131</v>
       </c>
       <c r="R188" s="5" t="s">
         <v>507</v>
@@ -18926,7 +18942,7 @@
         <v>2301</v>
       </c>
       <c r="Y188" s="5" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="Z188" s="5" t="s">
         <v>108</v>
@@ -18938,30 +18954,30 @@
         <v>0</v>
       </c>
       <c r="AC188" s="11">
-        <v>1.04162557e6</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AD188" s="11">
-        <v>1.04162557e6</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AE188" s="12">
-        <v>1.04162557e6</v>
+        <v>4.35942886e6</v>
       </c>
       <c r="AF188" s="12">
-        <v>1.04162557e6</v>
+        <v>4.35942886e6</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A189" s="13" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B189" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C189" s="14">
-        <v>43963</v>
+        <v>43935</v>
       </c>
       <c r="D189" s="15" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E189" s="15" t="s">
         <v>33</v>
@@ -18970,7 +18986,7 @@
         <v>2300</v>
       </c>
       <c r="G189" s="13" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="H189" s="13" t="s">
         <v>36</v>
@@ -18979,34 +18995,34 @@
         <v>37</v>
       </c>
       <c r="J189" s="17">
-        <v>9.247198e6</v>
+        <v>9.24595e6</v>
       </c>
       <c r="K189" s="15" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="L189" s="17">
         <v>2300</v>
       </c>
       <c r="M189" s="15" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="N189" s="18">
-        <v>43963</v>
+        <v>43936</v>
       </c>
       <c r="O189" s="18">
-        <v>43963</v>
+        <v>43936</v>
       </c>
       <c r="P189" s="19">
-        <v>44195</v>
+        <v>44119</v>
       </c>
       <c r="Q189" s="18">
-        <v>44195</v>
+        <v>44119</v>
       </c>
       <c r="R189" s="15" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="S189" s="15" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="T189" s="13" t="s">
         <v>33</v>
@@ -19024,7 +19040,7 @@
         <v>2301</v>
       </c>
       <c r="Y189" s="15" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="Z189" s="15" t="s">
         <v>108</v>
@@ -19036,39 +19052,39 @@
         <v>0</v>
       </c>
       <c r="AC189" s="22">
-        <v>7.11634326e6</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AD189" s="22">
-        <v>7.11634326e6</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AE189" s="23">
-        <v>7.11634326e6</v>
+        <v>1.04162557e6</v>
       </c>
       <c r="AF189" s="23">
-        <v>7.11634326e6</v>
+        <v>1.04162557e6</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A190" s="3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B190" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C190" s="4">
-        <v>43928</v>
+        <v>43963</v>
       </c>
       <c r="D190" s="5" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E190" s="5" t="s">
         <v>33</v>
       </c>
       <c r="F190" s="6">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="H190" s="3" t="s">
         <v>36</v>
@@ -19077,34 +19093,34 @@
         <v>37</v>
       </c>
       <c r="J190" s="7">
-        <v>9.245982e6</v>
+        <v>9.247198e6</v>
       </c>
       <c r="K190" s="5" t="s">
         <v>517</v>
       </c>
       <c r="L190" s="7">
-        <v>2310</v>
+        <v>2300</v>
       </c>
       <c r="M190" s="5" t="s">
-        <v>516</v>
+        <v>505</v>
       </c>
       <c r="N190" s="8">
-        <v>43943</v>
+        <v>43963</v>
       </c>
       <c r="O190" s="8">
-        <v>43939</v>
+        <v>43963</v>
       </c>
       <c r="P190" s="9">
-        <v>44304</v>
+        <v>44195</v>
       </c>
       <c r="Q190" s="8">
-        <v>44121</v>
+        <v>44195</v>
       </c>
       <c r="R190" s="5" t="s">
-        <v>425</v>
+        <v>518</v>
       </c>
       <c r="S190" s="5" t="s">
-        <v>426</v>
+        <v>519</v>
       </c>
       <c r="T190" s="3" t="s">
         <v>33</v>
@@ -19113,42 +19129,42 @@
         <v>33</v>
       </c>
       <c r="V190" s="7">
-        <v>18228</v>
-      </c>
-      <c r="W190" s="24" t="s">
-        <v>518</v>
+        <v>1155</v>
+      </c>
+      <c r="W190" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="X190" s="7">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="Y190" s="5" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="Z190" s="5" t="s">
-        <v>180</v>
+        <v>108</v>
       </c>
       <c r="AA190" s="3" t="s">
-        <v>519</v>
+        <v>44</v>
       </c>
       <c r="AB190" s="10">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="AC190" s="11">
-        <v>36</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AD190" s="11">
-        <v>36</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AE190" s="12">
-        <v>7200</v>
+        <v>7.11634326e6</v>
       </c>
       <c r="AF190" s="12">
-        <v>7200</v>
+        <v>7.11634326e6</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A191" s="13" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B191" s="13" t="s">
         <v>33</v>
@@ -19157,7 +19173,7 @@
         <v>43928</v>
       </c>
       <c r="D191" s="15" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E191" s="15" t="s">
         <v>33</v>
@@ -19166,7 +19182,7 @@
         <v>2310</v>
       </c>
       <c r="G191" s="13" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H191" s="13" t="s">
         <v>36</v>
@@ -19178,13 +19194,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K191" s="15" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L191" s="17">
         <v>2310</v>
       </c>
       <c r="M191" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N191" s="18">
         <v>43943</v>
@@ -19211,42 +19227,42 @@
         <v>33</v>
       </c>
       <c r="V191" s="17">
-        <v>236268</v>
-      </c>
-      <c r="W191" s="15" t="s">
-        <v>520</v>
+        <v>18228</v>
+      </c>
+      <c r="W191" s="20" t="s">
+        <v>524</v>
       </c>
       <c r="X191" s="17">
         <v>2311</v>
       </c>
       <c r="Y191" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z191" s="15" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="AA191" s="13" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB191" s="21">
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="AC191" s="22">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AD191" s="22">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="AE191" s="23">
-        <v>2250</v>
+        <v>7200</v>
       </c>
       <c r="AF191" s="23">
-        <v>2250</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A192" s="3" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B192" s="3" t="s">
         <v>33</v>
@@ -19255,7 +19271,7 @@
         <v>43928</v>
       </c>
       <c r="D192" s="5" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E192" s="5" t="s">
         <v>33</v>
@@ -19264,7 +19280,7 @@
         <v>2310</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H192" s="3" t="s">
         <v>36</v>
@@ -19276,13 +19292,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K192" s="5" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L192" s="7">
         <v>2310</v>
       </c>
       <c r="M192" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N192" s="8">
         <v>43943</v>
@@ -19309,42 +19325,42 @@
         <v>33</v>
       </c>
       <c r="V192" s="7">
-        <v>461920</v>
+        <v>236268</v>
       </c>
       <c r="W192" s="5" t="s">
-        <v>432</v>
+        <v>526</v>
       </c>
       <c r="X192" s="7">
         <v>2311</v>
       </c>
       <c r="Y192" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z192" s="5" t="s">
         <v>122</v>
       </c>
       <c r="AA192" s="3" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB192" s="10">
-        <v>600</v>
+        <v>50</v>
       </c>
       <c r="AC192" s="11">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AD192" s="11">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="AE192" s="12">
-        <v>4800</v>
+        <v>2250</v>
       </c>
       <c r="AF192" s="12">
-        <v>4800</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A193" s="13" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B193" s="13" t="s">
         <v>33</v>
@@ -19353,7 +19369,7 @@
         <v>43928</v>
       </c>
       <c r="D193" s="15" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E193" s="15" t="s">
         <v>33</v>
@@ -19362,7 +19378,7 @@
         <v>2310</v>
       </c>
       <c r="G193" s="13" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H193" s="13" t="s">
         <v>36</v>
@@ -19374,13 +19390,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K193" s="15" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L193" s="17">
         <v>2310</v>
       </c>
       <c r="M193" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N193" s="18">
         <v>43943</v>
@@ -19407,42 +19423,42 @@
         <v>33</v>
       </c>
       <c r="V193" s="17">
-        <v>804495</v>
+        <v>461920</v>
       </c>
       <c r="W193" s="15" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="X193" s="17">
         <v>2311</v>
       </c>
       <c r="Y193" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z193" s="15" t="s">
         <v>122</v>
       </c>
       <c r="AA193" s="13" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB193" s="21">
-        <v>170</v>
+        <v>600</v>
       </c>
       <c r="AC193" s="22">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AD193" s="22">
-        <v>45</v>
+        <v>8</v>
       </c>
       <c r="AE193" s="23">
-        <v>7650</v>
+        <v>4800</v>
       </c>
       <c r="AF193" s="23">
-        <v>7650</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A194" s="3" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B194" s="3" t="s">
         <v>33</v>
@@ -19451,7 +19467,7 @@
         <v>43928</v>
       </c>
       <c r="D194" s="5" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>33</v>
@@ -19460,7 +19476,7 @@
         <v>2310</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H194" s="3" t="s">
         <v>36</v>
@@ -19472,13 +19488,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K194" s="5" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L194" s="7">
         <v>2310</v>
       </c>
       <c r="M194" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N194" s="8">
         <v>43943</v>
@@ -19505,25 +19521,25 @@
         <v>33</v>
       </c>
       <c r="V194" s="7">
-        <v>1.129139e6</v>
+        <v>804495</v>
       </c>
       <c r="W194" s="5" t="s">
-        <v>521</v>
+        <v>427</v>
       </c>
       <c r="X194" s="7">
         <v>2311</v>
       </c>
       <c r="Y194" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z194" s="5" t="s">
         <v>122</v>
       </c>
       <c r="AA194" s="3" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB194" s="10">
-        <v>30</v>
+        <v>170</v>
       </c>
       <c r="AC194" s="11">
         <v>45</v>
@@ -19532,15 +19548,15 @@
         <v>45</v>
       </c>
       <c r="AE194" s="12">
-        <v>1350</v>
+        <v>7650</v>
       </c>
       <c r="AF194" s="12">
-        <v>1350</v>
+        <v>7650</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A195" s="13" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B195" s="13" t="s">
         <v>33</v>
@@ -19549,7 +19565,7 @@
         <v>43928</v>
       </c>
       <c r="D195" s="15" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E195" s="15" t="s">
         <v>33</v>
@@ -19558,7 +19574,7 @@
         <v>2310</v>
       </c>
       <c r="G195" s="13" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H195" s="13" t="s">
         <v>36</v>
@@ -19570,13 +19586,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K195" s="15" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L195" s="17">
         <v>2310</v>
       </c>
       <c r="M195" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N195" s="18">
         <v>43943</v>
@@ -19603,22 +19619,22 @@
         <v>33</v>
       </c>
       <c r="V195" s="17">
-        <v>1.152823e6</v>
+        <v>1.129139e6</v>
       </c>
       <c r="W195" s="15" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="X195" s="17">
         <v>2311</v>
       </c>
       <c r="Y195" s="15" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z195" s="15" t="s">
         <v>122</v>
       </c>
       <c r="AA195" s="13" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB195" s="21">
         <v>30</v>
@@ -19638,7 +19654,7 @@
     </row>
     <row r="196" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A196" s="3" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="B196" s="3" t="s">
         <v>33</v>
@@ -19647,7 +19663,7 @@
         <v>43928</v>
       </c>
       <c r="D196" s="5" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="E196" s="5" t="s">
         <v>33</v>
@@ -19656,7 +19672,7 @@
         <v>2310</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="H196" s="3" t="s">
         <v>36</v>
@@ -19668,13 +19684,13 @@
         <v>9.245982e6</v>
       </c>
       <c r="K196" s="5" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L196" s="7">
         <v>2310</v>
       </c>
       <c r="M196" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="N196" s="8">
         <v>43943</v>
@@ -19701,22 +19717,22 @@
         <v>33</v>
       </c>
       <c r="V196" s="7">
-        <v>1.152831e6</v>
+        <v>1.152823e6</v>
       </c>
       <c r="W196" s="5" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="X196" s="7">
         <v>2311</v>
       </c>
       <c r="Y196" s="5" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="Z196" s="5" t="s">
         <v>122</v>
       </c>
       <c r="AA196" s="3" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="AB196" s="10">
         <v>30</v>
@@ -19736,25 +19752,25 @@
     </row>
     <row r="197" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A197" s="13" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B197" s="13" t="s">
         <v>33</v>
       </c>
       <c r="C197" s="14">
-        <v>43944</v>
-      </c>
-      <c r="D197" s="25" t="s">
-        <v>525</v>
+        <v>43928</v>
+      </c>
+      <c r="D197" s="15" t="s">
+        <v>521</v>
       </c>
       <c r="E197" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F197" s="16">
-        <v>2320</v>
+        <v>2310</v>
       </c>
       <c r="G197" s="13" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="H197" s="13" t="s">
         <v>36</v>
@@ -19763,20 +19779,34 @@
         <v>37</v>
       </c>
       <c r="J197" s="17">
-        <v>0</v>
-      </c>
-      <c r="K197" s="15"/>
-      <c r="L197" s="17"/>
-      <c r="M197" s="15"/>
-      <c r="N197" s="18"/>
-      <c r="O197" s="18"/>
-      <c r="P197" s="19"/>
-      <c r="Q197" s="18"/>
+        <v>9.245982e6</v>
+      </c>
+      <c r="K197" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="L197" s="17">
+        <v>2310</v>
+      </c>
+      <c r="M197" s="15" t="s">
+        <v>522</v>
+      </c>
+      <c r="N197" s="18">
+        <v>43943</v>
+      </c>
+      <c r="O197" s="18">
+        <v>43939</v>
+      </c>
+      <c r="P197" s="19">
+        <v>44304</v>
+      </c>
+      <c r="Q197" s="18">
+        <v>44121</v>
+      </c>
       <c r="R197" s="15" t="s">
-        <v>527</v>
+        <v>425</v>
       </c>
       <c r="S197" s="15" t="s">
-        <v>528</v>
+        <v>426</v>
       </c>
       <c r="T197" s="13" t="s">
         <v>33</v>
@@ -19785,42 +19815,42 @@
         <v>33</v>
       </c>
       <c r="V197" s="17">
-        <v>1.692143e6</v>
+        <v>1.152831e6</v>
       </c>
       <c r="W197" s="15" t="s">
         <v>529</v>
       </c>
       <c r="X197" s="17">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="Y197" s="15" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="Z197" s="15" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="AA197" s="13" t="s">
-        <v>327</v>
+        <v>525</v>
       </c>
       <c r="AB197" s="21">
-        <v>3000</v>
+        <v>30</v>
       </c>
       <c r="AC197" s="22">
-        <v>8.2</v>
+        <v>45</v>
       </c>
       <c r="AD197" s="22">
-        <v>8.2</v>
+        <v>45</v>
       </c>
       <c r="AE197" s="23">
-        <v>24600</v>
+        <v>1350</v>
       </c>
       <c r="AF197" s="23">
-        <v>24600</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A198" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B198" s="3" t="s">
         <v>33</v>
@@ -19829,7 +19859,7 @@
         <v>43944</v>
       </c>
       <c r="D198" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E198" s="5" t="s">
         <v>33</v>
@@ -19838,7 +19868,7 @@
         <v>2320</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H198" s="3" t="s">
         <v>36</v>
@@ -19857,10 +19887,10 @@
       <c r="P198" s="9"/>
       <c r="Q198" s="8"/>
       <c r="R198" s="5" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="S198" s="5" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="T198" s="3" t="s">
         <v>33</v>
@@ -19869,42 +19899,42 @@
         <v>33</v>
       </c>
       <c r="V198" s="7">
-        <v>1.143883e6</v>
+        <v>1.692143e6</v>
       </c>
       <c r="W198" s="5" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="X198" s="7">
         <v>2321</v>
       </c>
       <c r="Y198" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z198" s="5" t="s">
-        <v>438</v>
+        <v>135</v>
       </c>
       <c r="AA198" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB198" s="10">
-        <v>200000</v>
+        <v>3000</v>
       </c>
       <c r="AC198" s="11">
-        <v>600000e-6</v>
+        <v>8.2</v>
       </c>
       <c r="AD198" s="11">
-        <v>600000e-6</v>
+        <v>8.2</v>
       </c>
       <c r="AE198" s="12">
-        <v>120000</v>
+        <v>24600</v>
       </c>
       <c r="AF198" s="12">
-        <v>120000</v>
+        <v>24600</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A199" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B199" s="13" t="s">
         <v>33</v>
@@ -19913,7 +19943,7 @@
         <v>43944</v>
       </c>
       <c r="D199" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E199" s="15" t="s">
         <v>33</v>
@@ -19922,7 +19952,7 @@
         <v>2320</v>
       </c>
       <c r="G199" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H199" s="13" t="s">
         <v>36</v>
@@ -19941,10 +19971,10 @@
       <c r="P199" s="19"/>
       <c r="Q199" s="18"/>
       <c r="R199" s="15" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="S199" s="15" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="T199" s="13" t="s">
         <v>33</v>
@@ -19953,42 +19983,42 @@
         <v>33</v>
       </c>
       <c r="V199" s="17">
-        <v>1.244515e6</v>
+        <v>1.143883e6</v>
       </c>
       <c r="W199" s="15" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="X199" s="17">
         <v>2321</v>
       </c>
       <c r="Y199" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z199" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA199" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB199" s="21">
-        <v>50</v>
+        <v>200000</v>
       </c>
       <c r="AC199" s="22">
-        <v>20.1</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD199" s="22">
-        <v>20.1</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE199" s="23">
-        <v>1005</v>
+        <v>120000</v>
       </c>
       <c r="AF199" s="23">
-        <v>1005</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A200" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B200" s="3" t="s">
         <v>33</v>
@@ -19997,7 +20027,7 @@
         <v>43944</v>
       </c>
       <c r="D200" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E200" s="5" t="s">
         <v>33</v>
@@ -20006,7 +20036,7 @@
         <v>2320</v>
       </c>
       <c r="G200" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H200" s="3" t="s">
         <v>36</v>
@@ -20025,10 +20055,10 @@
       <c r="P200" s="9"/>
       <c r="Q200" s="8"/>
       <c r="R200" s="5" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="S200" s="5" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="T200" s="3" t="s">
         <v>33</v>
@@ -20037,42 +20067,42 @@
         <v>33</v>
       </c>
       <c r="V200" s="7">
-        <v>1.244108e6</v>
+        <v>1.244515e6</v>
       </c>
       <c r="W200" s="5" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="X200" s="7">
         <v>2321</v>
       </c>
       <c r="Y200" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z200" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA200" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB200" s="10">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="AC200" s="11">
-        <v>358.24</v>
+        <v>20.1</v>
       </c>
       <c r="AD200" s="11">
-        <v>358.24</v>
+        <v>20.1</v>
       </c>
       <c r="AE200" s="12">
-        <v>32241.6</v>
+        <v>1005</v>
       </c>
       <c r="AF200" s="12">
-        <v>32241.6</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A201" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B201" s="13" t="s">
         <v>33</v>
@@ -20081,7 +20111,7 @@
         <v>43944</v>
       </c>
       <c r="D201" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E201" s="15" t="s">
         <v>33</v>
@@ -20090,7 +20120,7 @@
         <v>2320</v>
       </c>
       <c r="G201" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H201" s="13" t="s">
         <v>36</v>
@@ -20109,10 +20139,10 @@
       <c r="P201" s="19"/>
       <c r="Q201" s="18"/>
       <c r="R201" s="15" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S201" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T201" s="13" t="s">
         <v>33</v>
@@ -20121,42 +20151,42 @@
         <v>33</v>
       </c>
       <c r="V201" s="17">
-        <v>1.244507e6</v>
+        <v>1.244108e6</v>
       </c>
       <c r="W201" s="15" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="X201" s="17">
         <v>2321</v>
       </c>
       <c r="Y201" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z201" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA201" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB201" s="21">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="AC201" s="22">
-        <v>34.9</v>
+        <v>358.24</v>
       </c>
       <c r="AD201" s="22">
-        <v>34.9</v>
+        <v>358.24</v>
       </c>
       <c r="AE201" s="23">
-        <v>1745</v>
+        <v>32241.6</v>
       </c>
       <c r="AF201" s="23">
-        <v>1745</v>
+        <v>32241.6</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A202" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B202" s="3" t="s">
         <v>33</v>
@@ -20165,7 +20195,7 @@
         <v>43944</v>
       </c>
       <c r="D202" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E202" s="5" t="s">
         <v>33</v>
@@ -20174,7 +20204,7 @@
         <v>2320</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H202" s="3" t="s">
         <v>36</v>
@@ -20193,10 +20223,10 @@
       <c r="P202" s="9"/>
       <c r="Q202" s="8"/>
       <c r="R202" s="5" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S202" s="5" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T202" s="3" t="s">
         <v>33</v>
@@ -20205,42 +20235,42 @@
         <v>33</v>
       </c>
       <c r="V202" s="7">
-        <v>1.257587e6</v>
+        <v>1.244507e6</v>
       </c>
       <c r="W202" s="5" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="X202" s="7">
         <v>2321</v>
       </c>
       <c r="Y202" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z202" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA202" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB202" s="10">
-        <v>80000</v>
+        <v>50</v>
       </c>
       <c r="AC202" s="11">
-        <v>390000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AD202" s="11">
-        <v>390000e-6</v>
+        <v>34.9</v>
       </c>
       <c r="AE202" s="12">
-        <v>31200</v>
+        <v>1745</v>
       </c>
       <c r="AF202" s="12">
-        <v>31200</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A203" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B203" s="13" t="s">
         <v>33</v>
@@ -20249,7 +20279,7 @@
         <v>43944</v>
       </c>
       <c r="D203" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E203" s="15" t="s">
         <v>33</v>
@@ -20258,7 +20288,7 @@
         <v>2320</v>
       </c>
       <c r="G203" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H203" s="13" t="s">
         <v>36</v>
@@ -20277,10 +20307,10 @@
       <c r="P203" s="19"/>
       <c r="Q203" s="18"/>
       <c r="R203" s="15" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S203" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T203" s="13" t="s">
         <v>33</v>
@@ -20289,42 +20319,42 @@
         <v>33</v>
       </c>
       <c r="V203" s="17">
-        <v>1.257625e6</v>
+        <v>1.257587e6</v>
       </c>
       <c r="W203" s="15" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="X203" s="17">
         <v>2321</v>
       </c>
       <c r="Y203" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z203" s="15" t="s">
-        <v>387</v>
+        <v>444</v>
       </c>
       <c r="AA203" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB203" s="21">
-        <v>90</v>
+        <v>80000</v>
       </c>
       <c r="AC203" s="22">
-        <v>351</v>
+        <v>390000e-6</v>
       </c>
       <c r="AD203" s="22">
-        <v>351</v>
+        <v>390000e-6</v>
       </c>
       <c r="AE203" s="23">
-        <v>31590</v>
+        <v>31200</v>
       </c>
       <c r="AF203" s="23">
-        <v>31590</v>
+        <v>31200</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A204" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B204" s="3" t="s">
         <v>33</v>
@@ -20333,7 +20363,7 @@
         <v>43944</v>
       </c>
       <c r="D204" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E204" s="5" t="s">
         <v>33</v>
@@ -20342,7 +20372,7 @@
         <v>2320</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H204" s="3" t="s">
         <v>36</v>
@@ -20361,10 +20391,10 @@
       <c r="P204" s="9"/>
       <c r="Q204" s="8"/>
       <c r="R204" s="5" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S204" s="5" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T204" s="3" t="s">
         <v>33</v>
@@ -20373,42 +20403,42 @@
         <v>33</v>
       </c>
       <c r="V204" s="7">
-        <v>1.258699e6</v>
+        <v>1.257625e6</v>
       </c>
       <c r="W204" s="5" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="X204" s="7">
         <v>2321</v>
       </c>
       <c r="Y204" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z204" s="5" t="s">
-        <v>438</v>
+        <v>387</v>
       </c>
       <c r="AA204" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB204" s="10">
-        <v>2000</v>
+        <v>90</v>
       </c>
       <c r="AC204" s="11">
-        <v>1.39</v>
+        <v>351</v>
       </c>
       <c r="AD204" s="11">
-        <v>1.39</v>
+        <v>351</v>
       </c>
       <c r="AE204" s="12">
-        <v>2780</v>
+        <v>31590</v>
       </c>
       <c r="AF204" s="12">
-        <v>2780</v>
+        <v>31590</v>
       </c>
     </row>
     <row r="205" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A205" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B205" s="13" t="s">
         <v>33</v>
@@ -20417,7 +20447,7 @@
         <v>43944</v>
       </c>
       <c r="D205" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E205" s="15" t="s">
         <v>33</v>
@@ -20426,7 +20456,7 @@
         <v>2320</v>
       </c>
       <c r="G205" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H205" s="13" t="s">
         <v>36</v>
@@ -20445,10 +20475,10 @@
       <c r="P205" s="19"/>
       <c r="Q205" s="18"/>
       <c r="R205" s="15" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S205" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T205" s="13" t="s">
         <v>33</v>
@@ -20457,42 +20487,42 @@
         <v>33</v>
       </c>
       <c r="V205" s="17">
-        <v>1.259784e6</v>
+        <v>1.258699e6</v>
       </c>
       <c r="W205" s="15" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="X205" s="17">
         <v>2321</v>
       </c>
       <c r="Y205" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z205" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA205" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB205" s="21">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="AC205" s="22">
-        <v>600000e-6</v>
+        <v>1.39</v>
       </c>
       <c r="AD205" s="22">
-        <v>600000e-6</v>
+        <v>1.39</v>
       </c>
       <c r="AE205" s="23">
-        <v>1800</v>
+        <v>2780</v>
       </c>
       <c r="AF205" s="23">
-        <v>1800</v>
+        <v>2780</v>
       </c>
     </row>
     <row r="206" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A206" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B206" s="3" t="s">
         <v>33</v>
@@ -20501,7 +20531,7 @@
         <v>43944</v>
       </c>
       <c r="D206" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E206" s="5" t="s">
         <v>33</v>
@@ -20510,7 +20540,7 @@
         <v>2320</v>
       </c>
       <c r="G206" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H206" s="3" t="s">
         <v>36</v>
@@ -20529,10 +20559,10 @@
       <c r="P206" s="9"/>
       <c r="Q206" s="8"/>
       <c r="R206" s="5" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S206" s="5" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T206" s="3" t="s">
         <v>33</v>
@@ -20541,42 +20571,42 @@
         <v>33</v>
       </c>
       <c r="V206" s="7">
-        <v>1.259792e6</v>
+        <v>1.259784e6</v>
       </c>
       <c r="W206" s="5" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="X206" s="7">
         <v>2321</v>
       </c>
       <c r="Y206" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z206" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA206" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB206" s="10">
-        <v>80</v>
+        <v>3000</v>
       </c>
       <c r="AC206" s="11">
-        <v>15.35</v>
+        <v>600000e-6</v>
       </c>
       <c r="AD206" s="11">
-        <v>15.35</v>
+        <v>600000e-6</v>
       </c>
       <c r="AE206" s="12">
-        <v>1228</v>
+        <v>1800</v>
       </c>
       <c r="AF206" s="12">
-        <v>1228</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="207" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A207" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B207" s="13" t="s">
         <v>33</v>
@@ -20585,7 +20615,7 @@
         <v>43944</v>
       </c>
       <c r="D207" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E207" s="15" t="s">
         <v>33</v>
@@ -20594,7 +20624,7 @@
         <v>2320</v>
       </c>
       <c r="G207" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H207" s="13" t="s">
         <v>36</v>
@@ -20613,10 +20643,10 @@
       <c r="P207" s="19"/>
       <c r="Q207" s="18"/>
       <c r="R207" s="15" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S207" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T207" s="13" t="s">
         <v>33</v>
@@ -20625,42 +20655,42 @@
         <v>33</v>
       </c>
       <c r="V207" s="17">
-        <v>1.260669e6</v>
+        <v>1.259792e6</v>
       </c>
       <c r="W207" s="15" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="X207" s="17">
         <v>2321</v>
       </c>
       <c r="Y207" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z207" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA207" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB207" s="21">
-        <v>1000</v>
+        <v>80</v>
       </c>
       <c r="AC207" s="22">
-        <v>1.49</v>
+        <v>15.35</v>
       </c>
       <c r="AD207" s="22">
-        <v>1.49</v>
+        <v>15.35</v>
       </c>
       <c r="AE207" s="23">
-        <v>1490</v>
+        <v>1228</v>
       </c>
       <c r="AF207" s="23">
-        <v>1490</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="208" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A208" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B208" s="3" t="s">
         <v>33</v>
@@ -20669,7 +20699,7 @@
         <v>43944</v>
       </c>
       <c r="D208" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E208" s="5" t="s">
         <v>33</v>
@@ -20678,7 +20708,7 @@
         <v>2320</v>
       </c>
       <c r="G208" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H208" s="3" t="s">
         <v>36</v>
@@ -20697,10 +20727,10 @@
       <c r="P208" s="9"/>
       <c r="Q208" s="8"/>
       <c r="R208" s="5" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S208" s="5" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T208" s="3" t="s">
         <v>33</v>
@@ -20709,42 +20739,42 @@
         <v>33</v>
       </c>
       <c r="V208" s="7">
-        <v>1.260677e6</v>
+        <v>1.260669e6</v>
       </c>
       <c r="W208" s="5" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="X208" s="7">
         <v>2321</v>
       </c>
       <c r="Y208" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z208" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA208" s="3" t="s">
         <v>327</v>
       </c>
       <c r="AB208" s="10">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="AC208" s="11">
-        <v>1.59</v>
+        <v>1.49</v>
       </c>
       <c r="AD208" s="11">
-        <v>1.59</v>
+        <v>1.49</v>
       </c>
       <c r="AE208" s="12">
-        <v>4770</v>
+        <v>1490</v>
       </c>
       <c r="AF208" s="12">
-        <v>4770</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="209" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A209" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B209" s="13" t="s">
         <v>33</v>
@@ -20753,7 +20783,7 @@
         <v>43944</v>
       </c>
       <c r="D209" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E209" s="15" t="s">
         <v>33</v>
@@ -20762,7 +20792,7 @@
         <v>2320</v>
       </c>
       <c r="G209" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H209" s="13" t="s">
         <v>36</v>
@@ -20781,10 +20811,10 @@
       <c r="P209" s="19"/>
       <c r="Q209" s="18"/>
       <c r="R209" s="15" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S209" s="15" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T209" s="13" t="s">
         <v>33</v>
@@ -20793,42 +20823,42 @@
         <v>33</v>
       </c>
       <c r="V209" s="17">
-        <v>1.260731e6</v>
-      </c>
-      <c r="W209" s="20" t="s">
-        <v>548</v>
+        <v>1.260677e6</v>
+      </c>
+      <c r="W209" s="15" t="s">
+        <v>553</v>
       </c>
       <c r="X209" s="17">
         <v>2321</v>
       </c>
       <c r="Y209" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z209" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA209" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB209" s="21">
-        <v>60</v>
+        <v>3000</v>
       </c>
       <c r="AC209" s="22">
-        <v>271.97</v>
+        <v>1.59</v>
       </c>
       <c r="AD209" s="22">
-        <v>271.97</v>
+        <v>1.59</v>
       </c>
       <c r="AE209" s="23">
-        <v>16318.2</v>
+        <v>4770</v>
       </c>
       <c r="AF209" s="23">
-        <v>16318.2</v>
+        <v>4770</v>
       </c>
     </row>
     <row r="210" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A210" s="3" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>33</v>
@@ -20837,7 +20867,7 @@
         <v>43944</v>
       </c>
       <c r="D210" s="26" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E210" s="5" t="s">
         <v>33</v>
@@ -20846,7 +20876,7 @@
         <v>2320</v>
       </c>
       <c r="G210" s="3" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H210" s="3" t="s">
         <v>36</v>
@@ -20865,10 +20895,10 @@
       <c r="P210" s="9"/>
       <c r="Q210" s="8"/>
       <c r="R210" s="5" t="s">
-        <v>537</v>
+        <v>543</v>
       </c>
       <c r="S210" s="5" t="s">
-        <v>538</v>
+        <v>544</v>
       </c>
       <c r="T210" s="3" t="s">
         <v>33</v>
@@ -20877,19 +20907,19 @@
         <v>33</v>
       </c>
       <c r="V210" s="7">
-        <v>1.687115e6</v>
-      </c>
-      <c r="W210" s="5" t="s">
-        <v>549</v>
+        <v>1.260731e6</v>
+      </c>
+      <c r="W210" s="24" t="s">
+        <v>554</v>
       </c>
       <c r="X210" s="7">
         <v>2321</v>
       </c>
       <c r="Y210" s="5" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z210" s="5" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA210" s="3" t="s">
         <v>327</v>
@@ -20898,21 +20928,21 @@
         <v>60</v>
       </c>
       <c r="AC210" s="11">
-        <v>16.65</v>
+        <v>271.97</v>
       </c>
       <c r="AD210" s="11">
-        <v>16.65</v>
+        <v>271.97</v>
       </c>
       <c r="AE210" s="12">
-        <v>999</v>
+        <v>16318.2</v>
       </c>
       <c r="AF210" s="12">
-        <v>999</v>
+        <v>16318.2</v>
       </c>
     </row>
     <row r="211" s="1" customFormat="1" ht="18.1322" customHeight="1">
       <c r="A211" s="13" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B211" s="13" t="s">
         <v>33</v>
@@ -20921,7 +20951,7 @@
         <v>43944</v>
       </c>
       <c r="D211" s="25" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="E211" s="15" t="s">
         <v>33</v>
@@ -20930,7 +20960,7 @@
         <v>2320</v>
       </c>
       <c r="G211" s="13" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="H211" s="13" t="s">
         <v>36</v>
@@ -20949,10 +20979,10 @@
       <c r="P211" s="19"/>
       <c r="Q211" s="18"/>
       <c r="R211" s="15" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="S211" s="15" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="T211" s="13" t="s">
         <v>33</v>
@@ -20961,40 +20991,124 @@
         <v>33</v>
       </c>
       <c r="V211" s="17">
-        <v>1.257463e6</v>
+        <v>1.687115e6</v>
       </c>
       <c r="W211" s="15" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="X211" s="17">
         <v>2321</v>
       </c>
       <c r="Y211" s="15" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="Z211" s="15" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="AA211" s="13" t="s">
         <v>327</v>
       </c>
       <c r="AB211" s="21">
+        <v>60</v>
+      </c>
+      <c r="AC211" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AD211" s="22">
+        <v>16.65</v>
+      </c>
+      <c r="AE211" s="23">
+        <v>999</v>
+      </c>
+      <c r="AF211" s="23">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="212" s="1" customFormat="1" ht="18.1322" customHeight="1">
+      <c r="A212" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C212" s="4">
+        <v>43944</v>
+      </c>
+      <c r="D212" s="26" t="s">
+        <v>531</v>
+      </c>
+      <c r="E212" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F212" s="6">
+        <v>2320</v>
+      </c>
+      <c r="G212" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="H212" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I212" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J212" s="7">
+        <v>0</v>
+      </c>
+      <c r="K212" s="5"/>
+      <c r="L212" s="7"/>
+      <c r="M212" s="5"/>
+      <c r="N212" s="8"/>
+      <c r="O212" s="8"/>
+      <c r="P212" s="9"/>
+      <c r="Q212" s="8"/>
+      <c r="R212" s="5" t="s">
+        <v>556</v>
+      </c>
+      <c r="S212" s="5" t="s">
+        <v>557</v>
+      </c>
+      <c r="T212" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U212" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V212" s="7">
+        <v>1.257463e6</v>
+      </c>
+      <c r="W212" s="5" t="s">
+        <v>558</v>
+      </c>
+      <c r="X212" s="7">
+        <v>2321</v>
+      </c>
+      <c r="Y212" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z212" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="AA212" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="AB212" s="10">
         <v>200</v>
       </c>
-      <c r="AC211" s="22">
+      <c r="AC212" s="11">
         <v>34.2</v>
       </c>
-      <c r="AD211" s="22">
+      <c r="AD212" s="11">
         <v>34.2</v>
       </c>
-      <c r="AE211" s="23">
+      <c r="AE212" s="12">
         <v>6840</v>
       </c>
-      <c r="AF211" s="23">
+      <c r="AF212" s="12">
         <v>6840</v>
       </c>
     </row>
-    <row r="212" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
+    <row r="213" s="1" customFormat="1" ht="28.7982" customHeight="1"/>
   </sheetData>
   <pageSetup paperSize="9" scale="100" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>